<commit_message>
Add the predefined term table
</commit_message>
<xml_diff>
--- a/PredefinedTerms.xlsx
+++ b/PredefinedTerms.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mcamp\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GeoScripts\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD42D52F-AE9C-4141-938A-D86020B5C6DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A13DAB79-0C0C-4172-BAB8-C6043C8A3DE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="345" yWindow="1620" windowWidth="28800" windowHeight="11460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="PredefinedTerms" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>DatasetName</t>
   </si>
@@ -45,19 +45,10 @@
     <t>ParagraphStyle</t>
   </si>
   <si>
-    <t>GeoMaterialConfidence</t>
-  </si>
-  <si>
-    <t>Heading2</t>
-  </si>
-  <si>
-    <t>Low</t>
-  </si>
-  <si>
-    <t>Prepop test blah blah blah</t>
-  </si>
-  <si>
-    <t>2 Prepop 2 test 2  blah blah blah</t>
+    <t>Heading</t>
+  </si>
+  <si>
+    <t>Heading Definition</t>
   </si>
 </sst>
 </file>
@@ -375,10 +366,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -411,24 +402,10 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
         <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>